<commit_message>
Agregados más casos de prueba en el template
</commit_message>
<xml_diff>
--- a/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
+++ b/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Archivos Generales\Facultad\ISW\Repositorio\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D3E898-B94B-4432-8A0C-06040B533DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D09E057-EB25-41BE-B979-21F237BD26A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="147">
   <si>
     <t>TC_001</t>
   </si>
@@ -400,19 +400,6 @@
     <t>1. El usuario selecciona la opción "Lo Antes Posible".</t>
   </si>
   <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-2. El sistema valida que el usuario haya ingresado un monto válido para el pago, comprobando que "500" sea un número válido (mayor o igual al monto a pagar ("450"), y lo es.
-3. El sistema muestra el mensaje "¡Pedido realizado con éxito!".</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-2. El sistema valida que el número de tarjeta ingresado por el usuario "4755 1234 5678 9012" sea un número de tarjeta válido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y lo es.
-3. El sistema valida que el nombre y apellido ingresado por el usuario "Agustín Rodriguez" sea texto, válido y que corresponda con el número de la tarjeta ingresada, y lo es.
-4. El sistema valida que la fecha de vencimiento ingresada por el usuario "05/20" sea una fecha válida, con fecha mayor a la fecha actual, y lo es.
-5. El sistema valida que el código CVC ingresado por el usuario "598" sea un código numérico de 3 caracteres válidos, y lo es.
-6. El sistema muestra el mensaje "¡Pedido realizado con éxito!</t>
-  </si>
-  <si>
     <t>1. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
 2. El sistema muestra el mensaje "¡Su pedido se entregará lo antes posible!".</t>
   </si>
@@ -438,6 +425,116 @@
 2. El sistema valida que la fecha ingresada por el usuario "15/10/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y es así.
 3. El sistema valida que la hora ingresada por el usuario "22:00" sea una hora con formato válido, mayor a la hora actual, y es así.
 4. El sistema muestra el mensaje "¡Su pedido se entregará a la fecha y hora de recepción ingresadas!".</t>
+  </si>
+  <si>
+    <t>Registro de usuario con nombre de usuario existente.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Registrar Usuario".
+2. El usuario ingresa el nombre de usuario "pperez" para el registro del nuevo usuario.
+3. El usuario ingresa la dirección de correo "pperez@gmail.com".
+4. El usuario ingresa la contraseña "perez321".
+5. El usuario selecciona la opción "Registrar".</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para el registro del usuario.
+2. El sistema valida que el nombre de usuario "arodriguez" esté libre para su registro, y que el mismo posea al menos 8 caracteres, y no es así es así.
+3. El sistema muestra el mensaje "Nombre de usuario en uso. Ingrese otro".</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Forma de Pago: Efectivo con monto insuficiente</t>
+  </si>
+  <si>
+    <t>El usuario tiene que haber seleccionado previamente algún producto del comercio adherido, y haberlo agregado al carrito.
+El usuario tiene que haber llenado previamente los campos de dirección y ciudad.
+El monto a pagar es de $300.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la forma de pago "Efectivo".
+2. El usuario ingresa el monto a pagar "250".
+3. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+2. El sistema valida que el usuario haya ingresado un monto válido para el pago, comprobando que "500" sea un número válido (mayor o igual al monto a pagar ("450")), y lo es.
+3. El sistema muestra el mensaje "¡Pedido realizado con éxito!".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+2. El sistema valida que el usuario haya ingresado un monto válido para el pago, comprobando que "500" sea un número válido (mayor o igual al monto a pagar ("300")), y no lo es.
+3. El sistema muestra el mensaje "ERROR - Ingrese un monto superior al monto total de la compra.".</t>
+  </si>
+  <si>
+    <t>Forma de Pago: Tarjeta VISA con número de tarjeta inválido.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la forma de pago "Tarjeta VISA".
+2. El usuario ingresa el número de tarjeta "5258 1111 2222 3333".
+3. El usuario ingresa nombre y apellido "Pablo Pérez".
+4. El usuario ingresa fecha de vencimiento de la tarjeta "04/22".
+5. El usuario ingresa el CVC "198". 
+6. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+2. El sistema valida que el número de tarjeta ingresado por el usuario "5258 1111 2222 3333" sea un número de tarjeta válido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
+3. El sistema muestra el mensaje "El número de tarjeta no corresponde con una tarjeta VISA. Ingrese una tarjeta válida.".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+2. El sistema valida que el número de tarjeta ingresado por el usuario "4755 1234 5678 9012" sea un número de tarjeta válido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y lo es.
+3. El sistema valida que el nombre y apellido ingresado por el usuario "Agustín Rodriguez" sea texto, válido y que corresponda con el número de la tarjeta ingresada, y lo es.
+4. El sistema valida que la fecha de vencimiento ingresada por el usuario "05/20" sea una fecha válida, con fecha mayor a la fecha actual, y lo es.
+5. El sistema valida que el código CVC ingresado por el usuario "598" sea un código numérico de 3 caracteres válidos, y lo es.
+6. El sistema muestra el mensaje "¡Pedido realizado con éxito!"</t>
+  </si>
+  <si>
+    <t>Validación del momento de entrega seleccionado: "Fecha y Hora de Recepción" con fecha inválida.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Determinar fecha y hora de recepción".
+2. El usuario ingresa la fecha "10/09/2019" como fecha de recepción.
+3. El usuario ingresa la hora "22:00" como hora de recepción.
+4. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
+2. El sistema valida que la fecha ingresada por el usuario "10/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y no es así.
+3. El sistema muestra el mensaje "La fecha introducida es menor a la fecha actual. Ingrese una fecha válida para la recepción del pedido.".</t>
+  </si>
+  <si>
+    <t>Carrito de Productos</t>
+  </si>
+  <si>
+    <t>Visualización del carrito de compras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El usuario selecciona la opción de "Ver Carrito".
+</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla del carrito con los productos que se hayan agregado.</t>
+  </si>
+  <si>
+    <t>Fecha y Hora Estimada de Llegada</t>
+  </si>
+  <si>
+    <t>Visualización de la fecha y hora estimada de la llegada del pedido.</t>
+  </si>
+  <si>
+    <t>El usuario tiene que estar logueado con el Rol de "Comprador", tiene que haber seleccionado uno o más productos para que se hayan agregado al carrito de compras, y tiene que tener un pedido realizado.</t>
+  </si>
+  <si>
+    <t>El usuario tiene que estar logueado con el Rol de "Comprador", y tiene que haber seleccionado uno o más productos para que se hayan agregado al carrito de compras.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Ver mis pedidos".</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla del pedido con los productos del mismo, el monto total, la forma de pago elegida, y la fecha y hora estimada de llegada.</t>
   </si>
 </sst>
 </file>
@@ -1738,9 +1835,9 @@
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2134,27 +2231,27 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>92</v>
+        <v>100</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="15"/>
@@ -2178,27 +2275,27 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>94</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="15"/>
@@ -2230,19 +2327,19 @@
         <v>100</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>94</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="15"/>
@@ -2266,27 +2363,27 @@
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
     </row>
-    <row r="15" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="15"/>
@@ -2310,7 +2407,7 @@
       <c r="AR15" s="7"/>
       <c r="AS15" s="7"/>
     </row>
-    <row r="16" spans="1:45" ht="180" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -2321,16 +2418,16 @@
         <v>106</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="15"/>
@@ -2354,27 +2451,27 @@
       <c r="AR16" s="7"/>
       <c r="AS16" s="7"/>
     </row>
-    <row r="17" spans="1:45" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="15"/>
@@ -2398,7 +2495,7 @@
       <c r="AR17" s="7"/>
       <c r="AS17" s="7"/>
     </row>
-    <row r="18" spans="1:45" ht="120" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" ht="180" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>46</v>
       </c>
@@ -2406,19 +2503,19 @@
         <v>86</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="G18" s="26" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="15"/>
@@ -2442,16 +2539,28 @@
       <c r="AR18" s="7"/>
       <c r="AS18" s="7"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" ht="120" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+      <c r="B19" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>132</v>
+      </c>
       <c r="H19" s="26"/>
       <c r="I19" s="15"/>
       <c r="J19" s="28"/>
@@ -2474,16 +2583,28 @@
       <c r="AR19" s="7"/>
       <c r="AS19" s="7"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
+      <c r="B20" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>116</v>
+      </c>
       <c r="H20" s="26"/>
       <c r="I20" s="15"/>
       <c r="J20" s="28"/>
@@ -2506,16 +2627,28 @@
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" ht="120" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
+      <c r="B21" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>120</v>
+      </c>
       <c r="H21" s="26"/>
       <c r="I21" s="15"/>
       <c r="J21" s="28"/>
@@ -2538,16 +2671,28 @@
       <c r="AR21" s="7"/>
       <c r="AS21" s="7"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="B22" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>136</v>
+      </c>
       <c r="H22" s="26"/>
       <c r="I22" s="15"/>
       <c r="J22" s="28"/>
@@ -2570,16 +2715,28 @@
       <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="B23" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>140</v>
+      </c>
       <c r="H23" s="26"/>
       <c r="I23" s="15"/>
       <c r="J23" s="28"/>
@@ -2602,16 +2759,28 @@
       <c r="AR23" s="7"/>
       <c r="AS23" s="7"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="B24" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>146</v>
+      </c>
       <c r="H24" s="26"/>
       <c r="I24" s="15"/>
       <c r="J24" s="28"/>
@@ -2634,16 +2803,28 @@
       <c r="AR24" s="7"/>
       <c r="AS24" s="7"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="B25" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>146</v>
+      </c>
       <c r="H25" s="26"/>
       <c r="I25" s="15"/>
       <c r="J25" s="28"/>
@@ -4387,7 +4568,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I73 S12:S73 N12:N73 M11 R11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B73" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11 B17:B73" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4657,6 +4838,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -4782,24 +4980,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4815,22 +5014,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
datos cargados al template de casos de pprueba del grupo 6
</commit_message>
<xml_diff>
--- a/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
+++ b/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
@@ -1,35 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Archivos Generales\Facultad\ISW\Repositorio\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\UTN\Ingenieria de Software\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D09E057-EB25-41BE-B979-21F237BD26A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
     <sheet name="Bugs" sheetId="28" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Casos_Prueba!$A$9:$AS$2331</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Casos_Prueba!$A$9:$AS$2329</definedName>
     <definedName name="gr" localSheetId="0">#REF!</definedName>
     <definedName name="gr">#REF!</definedName>
     <definedName name="Ready_To_Run" localSheetId="0">#REF!</definedName>
     <definedName name="Ready_To_Run">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="160">
   <si>
     <t>TC_001</t>
   </si>
@@ -275,9 +274,6 @@
   </si>
   <si>
     <t>Descripción</t>
-  </si>
-  <si>
-    <t>Pasos para repruducirlo</t>
   </si>
   <si>
     <t>Severidad</t>
@@ -516,9 +512,6 @@
 </t>
   </si>
   <si>
-    <t>1. El sistema muestra la pantalla del carrito con los productos que se hayan agregado.</t>
-  </si>
-  <si>
     <t>Fecha y Hora Estimada de Llegada</t>
   </si>
   <si>
@@ -535,12 +528,58 @@
   </si>
   <si>
     <t>1. El sistema muestra la pantalla del pedido con los productos del mismo, el monto total, la forma de pago elegida, y la fecha y hora estimada de llegada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema muestra la pantalla del carrito con los productos que se hayan agregado. Los productos iguales no se muestran agrupados. </t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla del carrito con los productos que se hayan agregado. Los productos deben mostrarse agrupados por nombre nombre de producto.</t>
+  </si>
+  <si>
+    <t>Fallo</t>
+  </si>
+  <si>
+    <t>Los productos iguales no se muestran agrupados</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Ver mis pedidos"</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Ver mis pedidos".
+2. El usuario selecciona la opción 'editar' de un detalle del pedido.</t>
+  </si>
+  <si>
+    <t>Editar detalle de pedido</t>
+  </si>
+  <si>
+    <t>No se observan validaciones ni mensajes de alerta por parte del sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema no notifica si hay datos faltantes o si el pedido se registró con éxito por lo cual deja con incertidumbre al usuario acerca del estado del mismo. </t>
+  </si>
+  <si>
+    <t>Funcionalidad inaccesible</t>
+  </si>
+  <si>
+    <t>No es posible registrar un pedido exitosamente</t>
+  </si>
+  <si>
+    <t>Severo</t>
+  </si>
+  <si>
+    <t>Creado</t>
+  </si>
+  <si>
+    <t>Pasos para reproducirlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema no aparenta validar los campos de dirección </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1044,18 +1083,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="DataPilot Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="DataPilot Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="DataPilot Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="DataPilot Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="DataPilot Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="DataPilot Category" xfId="1"/>
+    <cellStyle name="DataPilot Corner" xfId="2"/>
+    <cellStyle name="DataPilot Field" xfId="3"/>
+    <cellStyle name="DataPilot Result" xfId="4"/>
+    <cellStyle name="DataPilot Title" xfId="5"/>
+    <cellStyle name="DataPilot Value" xfId="6"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 2" xfId="8"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="240">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1066,6 +1112,58 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -1102,6 +1200,1358 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1829,15 +3279,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS73"/>
+  <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2099,7 +3549,7 @@
         <v>66</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>67</v>
@@ -2187,42 +3637,52 @@
       <c r="AB10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="1:45" ht="144" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="F11" s="26" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" s="29">
+        <v>2</v>
+      </c>
+      <c r="L11" s="37">
+        <v>43753</v>
+      </c>
+      <c r="M11" s="39"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="29"/>
       <c r="V11" s="16"/>
       <c r="AN11" s="7"/>
       <c r="AO11" s="7"/>
@@ -2231,33 +3691,43 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="96" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>121</v>
+        <v>99</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="37"/>
+        <v>98</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K12" s="29">
+        <v>2</v>
+      </c>
+      <c r="L12" s="37">
+        <v>43753</v>
+      </c>
       <c r="M12" s="39"/>
       <c r="N12" s="15"/>
       <c r="O12" s="28"/>
@@ -2275,33 +3745,43 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>91</v>
-      </c>
       <c r="D13" s="21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="37"/>
+        <v>104</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K13" s="29">
+        <v>2</v>
+      </c>
+      <c r="L13" s="37">
+        <v>43753</v>
+      </c>
       <c r="M13" s="39"/>
       <c r="N13" s="15"/>
       <c r="O13" s="28"/>
@@ -2319,33 +3799,43 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="37"/>
+        <v>127</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="29">
+        <v>2</v>
+      </c>
+      <c r="L14" s="37">
+        <v>43753</v>
+      </c>
       <c r="M14" s="39"/>
       <c r="N14" s="15"/>
       <c r="O14" s="28"/>
@@ -2363,33 +3853,43 @@
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
     </row>
-    <row r="15" spans="1:45" ht="60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>102</v>
-      </c>
       <c r="E15" s="26" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="37"/>
+        <v>128</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K15" s="29">
+        <v>2</v>
+      </c>
+      <c r="L15" s="37">
+        <v>43753</v>
+      </c>
       <c r="M15" s="39"/>
       <c r="N15" s="15"/>
       <c r="O15" s="28"/>
@@ -2407,33 +3907,43 @@
       <c r="AR15" s="7"/>
       <c r="AS15" s="7"/>
     </row>
-    <row r="16" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="180" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="26" t="s">
-        <v>109</v>
-      </c>
       <c r="F16" s="26" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="37"/>
+        <v>132</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K16" s="29">
+        <v>2</v>
+      </c>
+      <c r="L16" s="37">
+        <v>43753</v>
+      </c>
       <c r="M16" s="39"/>
       <c r="N16" s="15"/>
       <c r="O16" s="28"/>
@@ -2451,33 +3961,43 @@
       <c r="AR16" s="7"/>
       <c r="AS16" s="7"/>
     </row>
-    <row r="17" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" ht="120" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="37"/>
+        <v>131</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K17" s="29">
+        <v>2</v>
+      </c>
+      <c r="L17" s="37">
+        <v>43753</v>
+      </c>
       <c r="M17" s="39"/>
       <c r="N17" s="15"/>
       <c r="O17" s="28"/>
@@ -2495,33 +4015,43 @@
       <c r="AR17" s="7"/>
       <c r="AS17" s="7"/>
     </row>
-    <row r="18" spans="1:45" ht="180" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="37"/>
+        <v>115</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K18" s="29">
+        <v>2</v>
+      </c>
+      <c r="L18" s="37">
+        <v>43753</v>
+      </c>
       <c r="M18" s="39"/>
       <c r="N18" s="15"/>
       <c r="O18" s="28"/>
@@ -2544,28 +4074,38 @@
         <v>47</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="37"/>
+        <v>119</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K19" s="29">
+        <v>2</v>
+      </c>
+      <c r="L19" s="37">
+        <v>43753</v>
+      </c>
       <c r="M19" s="39"/>
       <c r="N19" s="15"/>
       <c r="O19" s="28"/>
@@ -2583,33 +4123,43 @@
       <c r="AR19" s="7"/>
       <c r="AS19" s="7"/>
     </row>
-    <row r="20" spans="1:45" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C20" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>113</v>
-      </c>
       <c r="F20" s="26" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="37"/>
+        <v>135</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K20" s="29">
+        <v>2</v>
+      </c>
+      <c r="L20" s="37">
+        <v>43753</v>
+      </c>
       <c r="M20" s="39"/>
       <c r="N20" s="15"/>
       <c r="O20" s="28"/>
@@ -2627,33 +4177,43 @@
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
     </row>
-    <row r="21" spans="1:45" ht="120" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="37"/>
+        <v>146</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="K21" s="29">
+        <v>1</v>
+      </c>
+      <c r="L21" s="37">
+        <v>43753.45208333333</v>
+      </c>
       <c r="M21" s="39"/>
       <c r="N21" s="15"/>
       <c r="O21" s="28"/>
@@ -2671,33 +4231,43 @@
       <c r="AR21" s="7"/>
       <c r="AS21" s="7"/>
     </row>
-    <row r="22" spans="1:45" ht="96" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="37"/>
+        <v>144</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="K22" s="29">
+        <v>3</v>
+      </c>
+      <c r="L22" s="37">
+        <v>43753</v>
+      </c>
       <c r="M22" s="39"/>
       <c r="N22" s="15"/>
       <c r="O22" s="28"/>
@@ -2715,33 +4285,43 @@
       <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
     </row>
-    <row r="23" spans="1:45" ht="60" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E23" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="37"/>
+      <c r="H23" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="K23" s="29">
+        <v>3</v>
+      </c>
+      <c r="L23" s="37">
+        <v>43753</v>
+      </c>
       <c r="M23" s="39"/>
       <c r="N23" s="15"/>
       <c r="O23" s="28"/>
@@ -2764,23 +4344,21 @@
         <v>52</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>143</v>
-      </c>
       <c r="F24" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="G24" s="26" t="s">
-        <v>146</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="G24" s="26"/>
       <c r="H24" s="26"/>
       <c r="I24" s="15"/>
       <c r="J24" s="28"/>
@@ -2803,28 +4381,16 @@
       <c r="AR24" s="7"/>
       <c r="AS24" s="7"/>
     </row>
-    <row r="25" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="G25" s="26" t="s">
-        <v>146</v>
-      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="26"/>
       <c r="I25" s="15"/>
       <c r="J25" s="28"/>
@@ -4166,8 +5732,8 @@
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
       <c r="G67" s="26"/>
       <c r="H67" s="26"/>
       <c r="I67" s="15"/>
@@ -4198,8 +5764,8 @@
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
       <c r="D68" s="21"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="26"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
       <c r="G68" s="26"/>
       <c r="H68" s="26"/>
       <c r="I68" s="15"/>
@@ -4230,8 +5796,8 @@
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
       <c r="D69" s="21"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
       <c r="G69" s="26"/>
       <c r="H69" s="26"/>
       <c r="I69" s="15"/>
@@ -4262,8 +5828,8 @@
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
       <c r="D70" s="21"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
       <c r="G70" s="26"/>
       <c r="H70" s="26"/>
       <c r="I70" s="15"/>
@@ -4292,9 +5858,9 @@
         <v>37</v>
       </c>
       <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="26"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="22"/>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
       <c r="H71" s="26"/>
@@ -4319,72 +5885,8 @@
       <c r="AR71" s="7"/>
       <c r="AS71" s="7"/>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A72" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="26"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="26"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="28"/>
-      <c r="K72" s="29"/>
-      <c r="L72" s="37"/>
-      <c r="M72" s="39"/>
-      <c r="N72" s="15"/>
-      <c r="O72" s="28"/>
-      <c r="P72" s="29"/>
-      <c r="Q72" s="16"/>
-      <c r="R72" s="39"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="28"/>
-      <c r="U72" s="29"/>
-      <c r="V72" s="16"/>
-      <c r="AN72" s="7"/>
-      <c r="AO72" s="7"/>
-      <c r="AP72" s="7"/>
-      <c r="AQ72" s="7"/>
-      <c r="AR72" s="7"/>
-      <c r="AS72" s="7"/>
-    </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A73" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B73" s="21"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="26"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="28"/>
-      <c r="K73" s="29"/>
-      <c r="L73" s="37"/>
-      <c r="M73" s="39"/>
-      <c r="N73" s="15"/>
-      <c r="O73" s="28"/>
-      <c r="P73" s="29"/>
-      <c r="Q73" s="16"/>
-      <c r="R73" s="39"/>
-      <c r="S73" s="15"/>
-      <c r="T73" s="28"/>
-      <c r="U73" s="29"/>
-      <c r="V73" s="16"/>
-      <c r="AN73" s="7"/>
-      <c r="AO73" s="7"/>
-      <c r="AP73" s="7"/>
-      <c r="AQ73" s="7"/>
-      <c r="AR73" s="7"/>
-      <c r="AS73" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A9:AS2331" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A9:AS2329"/>
   <mergeCells count="7">
     <mergeCell ref="A2:F4"/>
     <mergeCell ref="H8:L8"/>
@@ -4394,181 +5896,419 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="D5:F5"/>
   </mergeCells>
-  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 O12:O606 J12:J606">
-    <cfRule type="cellIs" dxfId="46" priority="68" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="J621:J745 J747 J749 J751 J753 J755 J757 J759 J761 J763:J769 J917:J1040 J1042:J1179 J1184:J1198 J1203:J1207 J1212:J1261 J1265:J1289 J1291:J1383 J1387:J1411 J1413:J1472 J1474:J1560 J1599:J1620 J1757:J1758 J1761:J1788 J1916:J1957 J1960:J1962 J1965 J1967:J1969 J1972:J2009 J2012:J2052 J2055:J2077 J2080:J2083 J2086 J2088:J2090 J2093:J2134 J2330:J65042 O621:O745 O747 O749 O751 O753 O755 O757 O759 O761 O763:O769 O917:O1040 O1042:O1179 O1184:O1198 O1203:O1207 O1212:O1261 O1265:O1289 O1291:O1383 O1387:O1411 O1413:O1472 O1474:O1560 O1599:O1620 O1757:O1758 O1761:O1788 O1916:O1957 O1960:O1962 O1965 O1967:O1969 O1972:O2009 O2012:O2052 O2055:O2077 O2080:O2083 O2086 O2088:O2090 O2093:O2134 O2330:O65042 J21:J22 J24:J604 O9:O604 J9:J11 T11:T604">
+    <cfRule type="cellIs" dxfId="139" priority="168" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="169" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="170" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I73 N12:N73">
-    <cfRule type="cellIs" dxfId="43" priority="60" operator="equal">
+  <conditionalFormatting sqref="I21:I22 I24:I71 I11 N11:N71 S11:S71">
+    <cfRule type="cellIs" dxfId="136" priority="160" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="161" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="162" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="163" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="164" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I73 N12:N73">
-    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
+  <conditionalFormatting sqref="I21:I22 I24:I71 I11 N11:N71 S11:S71">
+    <cfRule type="cellIs" dxfId="131" priority="145" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="146" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T623:T747 T749 T751 T753 T755 T757 T759 T761 T763 T765:T771 T919:T1042 T1044:T1181 T1186:T1200 T1205:T1209 T1214:T1263 T1267:T1291 T1293:T1385 T1389:T1413 T1415:T1474 T1476:T1562 T1601:T1622 T1759:T1760 T1763:T1790 T1918:T1959 T1962:T1964 T1967 T1969:T1971 T1974:T2011 T2014:T2054 T2057:T2079 T2082:T2085 T2088 T2090:T2092 T2095:T2136 T2332:T65044 T9:T10 T12:T606">
-    <cfRule type="cellIs" dxfId="36" priority="35" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="T621:T745 T747 T749 T751 T753 T755 T757 T759 T761 T763:T769 T917:T1040 T1042:T1179 T1184:T1198 T1203:T1207 T1212:T1261 T1265:T1289 T1291:T1383 T1387:T1411 T1413:T1472 T1474:T1560 T1599:T1620 T1757:T1758 T1761:T1788 T1916:T1957 T1960:T1962 T1965 T1967:T1969 T1972:T2009 T2012:T2052 T2055:T2077 T2080:T2083 T2086 T2088:T2090 T2093:T2134 T2330:T65042 T9:T10">
+    <cfRule type="cellIs" dxfId="129" priority="135" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="136" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="137" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12:S73">
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+  <conditionalFormatting sqref="J12">
+    <cfRule type="cellIs" dxfId="99" priority="98" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="99" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="100" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="96" priority="93" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="94" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="96" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12:S73">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="26" priority="25" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="J13">
+    <cfRule type="cellIs" dxfId="89" priority="88" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="89" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="90" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="86" priority="83" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="84" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="86" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="87" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="J14">
+    <cfRule type="cellIs" dxfId="79" priority="78" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="79" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="80" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="76" priority="73" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="74" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="76" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="77" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+  <conditionalFormatting sqref="J15">
+    <cfRule type="cellIs" dxfId="69" priority="68" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="69" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="70" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="66" priority="63" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="66" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="cellIs" dxfId="59" priority="58" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="60" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="57" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="cellIs" dxfId="49" priority="48" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="49" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="50" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="cellIs" dxfId="39" priority="38" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="39" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="40" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="cellIs" dxfId="29" priority="28" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20">
+    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P67:P68 K67:K68 U67:U68" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I73 S12:S73 N12:N73 M11 R11" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P65:P66 K65:K66 U65:U66"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N11:N71 S11:S71 I11:I71">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11 B17:B73" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B15:B71">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4579,11 +6319,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H18"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4613,16 +6353,16 @@
         <v>80</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>81</v>
       </c>
       <c r="E2" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>82</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>83</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>66</v>
@@ -4646,43 +6386,61 @@
         <v>1</v>
       </c>
       <c r="B4" s="21"/>
-      <c r="C4" s="44"/>
+      <c r="C4" s="44">
+        <v>43753</v>
+      </c>
       <c r="D4" s="21"/>
       <c r="E4" s="26"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="F4" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>2</v>
       </c>
       <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="C5" s="44">
+        <v>43753</v>
+      </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="H5" s="21" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>3</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="C6" s="44">
+        <v>43753</v>
+      </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="H6" s="21" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>4</v>
       </c>
       <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="C7" s="44">
+        <v>43753</v>
+      </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
@@ -4694,7 +6452,9 @@
         <v>5</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="C8" s="44">
+        <v>43753</v>
+      </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -4706,7 +6466,9 @@
         <v>6</v>
       </c>
       <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
+      <c r="C9" s="44">
+        <v>43753</v>
+      </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -4718,7 +6480,9 @@
         <v>7</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="C10" s="44">
+        <v>43753</v>
+      </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
@@ -4730,7 +6494,9 @@
         <v>8</v>
       </c>
       <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
+      <c r="C11" s="44">
+        <v>43753</v>
+      </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -4823,13 +6589,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{C5E3F37E-FB36-4F7F-99E9-6282EDC122A6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4847,14 +6613,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -4980,6 +6738,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
@@ -4989,16 +6755,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5014,4 +6770,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualizada la planilla de casos de prueba
</commit_message>
<xml_diff>
--- a/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
+++ b/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\UTN\Ingenieria de Software\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Archivos Generales\Facultad\ISW\Repositorio\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043D7090-8883-4E8A-93B4-976CB209ED81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
     <sheet name="Bugs" sheetId="28" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Casos_Prueba!$A$9:$AS$2329</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Casos_Prueba!$A$9:$AS$2326</definedName>
     <definedName name="gr" localSheetId="0">#REF!</definedName>
     <definedName name="gr">#REF!</definedName>
     <definedName name="Ready_To_Run" localSheetId="0">#REF!</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="168">
   <si>
     <t>TC_001</t>
   </si>
@@ -135,21 +136,6 @@
     <t>TC_058</t>
   </si>
   <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
     <t>TC_002</t>
   </si>
   <si>
@@ -288,34 +274,10 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la opción "Registrar Usuario".
-2. El usuario ingresa el nombre de usuario "arodriguez" para el registro del nuevo usuario.
-3. El usuario ingresa la dirección de correo "arodriguez@gmail.com".
-4. El usuario ingresa la contraseña "user1234".
-5. El usuario selecciona la opción "Registrar".</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla para el registro del usuario.
-2. El sistema valida que el nombre de usuario "arodriguez" esté libre para su registro, y que el mismo posea al menos 8 caracteres, y es así.
-3. El sistema valida el formato de la dirección de correo "arodriguez@gmail.com", y es válida.
-4. El sistema valida que la contraseña "user1234" esté compuesta por al menos 8 caracteres alfanuméricos, y es así.
-5. El sistema valida muestra el mensaje "¡El usuario ha sido registrado exitosamente!
-6. El sistema registra un nuevo usuario con el nombre de usuario "arodriguez".</t>
-  </si>
-  <si>
-    <t>El celular del usuario tiene conexión a Internet, y el usuario cedió previamente permisos a la aplicación para que la misma haga uso de ésta.</t>
-  </si>
-  <si>
     <t>Dirección</t>
   </si>
   <si>
     <t>Validación de la dirección ingresada para pedido.</t>
-  </si>
-  <si>
-    <t>Registro de usuario.</t>
   </si>
   <si>
     <t>El usuario tiene que haber seleccionado previamente algún producto del comercio adherido, y haberlo agregado al carrito.</t>
@@ -374,11 +336,6 @@
     <t>El usuario tiene que haber seleccionado previamente algún producto del comercio adherido, y haberlo agregado al carrito.
 El usuario tiene que haber llenado previamente los campos de dirección y ciudad.
 El monto a pagar es de $450.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la forma de pago "Efectivo".
-2. El usuario ingresa el monto a pagar "500".
-3. El usuario selecciona la opción "Aceptar".</t>
   </si>
   <si>
     <t>Validación de la forma de pago seleccionada: Tarjeta VISA.</t>
@@ -423,61 +380,7 @@
 4. El sistema muestra el mensaje "¡Su pedido se entregará a la fecha y hora de recepción ingresadas!".</t>
   </si>
   <si>
-    <t>Registro de usuario con nombre de usuario existente.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la opción "Registrar Usuario".
-2. El usuario ingresa el nombre de usuario "pperez" para el registro del nuevo usuario.
-3. El usuario ingresa la dirección de correo "pperez@gmail.com".
-4. El usuario ingresa la contraseña "perez321".
-5. El usuario selecciona la opción "Registrar".</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla para el registro del usuario.
-2. El sistema valida que el nombre de usuario "arodriguez" esté libre para su registro, y que el mismo posea al menos 8 caracteres, y no es así es así.
-3. El sistema muestra el mensaje "Nombre de usuario en uso. Ingrese otro".</t>
-  </si>
-  <si>
     <t>Baja</t>
-  </si>
-  <si>
-    <t>Forma de Pago: Efectivo con monto insuficiente</t>
-  </si>
-  <si>
-    <t>El usuario tiene que haber seleccionado previamente algún producto del comercio adherido, y haberlo agregado al carrito.
-El usuario tiene que haber llenado previamente los campos de dirección y ciudad.
-El monto a pagar es de $300.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la forma de pago "Efectivo".
-2. El usuario ingresa el monto a pagar "250".
-3. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-2. El sistema valida que el usuario haya ingresado un monto válido para el pago, comprobando que "500" sea un número válido (mayor o igual al monto a pagar ("450")), y lo es.
-3. El sistema muestra el mensaje "¡Pedido realizado con éxito!".</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-2. El sistema valida que el usuario haya ingresado un monto válido para el pago, comprobando que "500" sea un número válido (mayor o igual al monto a pagar ("300")), y no lo es.
-3. El sistema muestra el mensaje "ERROR - Ingrese un monto superior al monto total de la compra.".</t>
-  </si>
-  <si>
-    <t>Forma de Pago: Tarjeta VISA con número de tarjeta inválido.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la forma de pago "Tarjeta VISA".
-2. El usuario ingresa el número de tarjeta "5258 1111 2222 3333".
-3. El usuario ingresa nombre y apellido "Pablo Pérez".
-4. El usuario ingresa fecha de vencimiento de la tarjeta "04/22".
-5. El usuario ingresa el CVC "198". 
-6. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-2. El sistema valida que el número de tarjeta ingresado por el usuario "5258 1111 2222 3333" sea un número de tarjeta válido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
-3. El sistema muestra el mensaje "El número de tarjeta no corresponde con una tarjeta VISA. Ingrese una tarjeta válida.".</t>
   </si>
   <si>
     <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
@@ -488,102 +391,239 @@
 6. El sistema muestra el mensaje "¡Pedido realizado con éxito!"</t>
   </si>
   <si>
-    <t>Validación del momento de entrega seleccionado: "Fecha y Hora de Recepción" con fecha inválida.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la opción "Determinar fecha y hora de recepción".
-2. El usuario ingresa la fecha "10/09/2019" como fecha de recepción.
-3. El usuario ingresa la hora "22:00" como hora de recepción.
-4. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
-2. El sistema valida que la fecha ingresada por el usuario "10/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y no es así.
-3. El sistema muestra el mensaje "La fecha introducida es menor a la fecha actual. Ingrese una fecha válida para la recepción del pedido.".</t>
-  </si>
-  <si>
     <t>Carrito de Productos</t>
   </si>
   <si>
     <t>Visualización del carrito de compras.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. El usuario selecciona la opción de "Ver Carrito".
+    <t>Fecha y Hora Estimada de Llegada</t>
+  </si>
+  <si>
+    <t>Visualización de la fecha y hora estimada de la llegada del pedido.</t>
+  </si>
+  <si>
+    <t>El usuario tiene que estar logueado con el Rol de "Comprador", tiene que haber seleccionado uno o más productos para que se hayan agregado al carrito de compras, y tiene que tener un pedido realizado.</t>
+  </si>
+  <si>
+    <t>El usuario tiene que estar logueado con el Rol de "Comprador", y tiene que haber seleccionado uno o más productos para que se hayan agregado al carrito de compras.</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla del pedido con los productos del mismo, el monto total, la forma de pago elegida, y la fecha y hora estimada de llegada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema muestra la pantalla del carrito con los productos que se hayan agregado. Los productos iguales no se muestran agrupados. </t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla del carrito con los productos que se hayan agregado. Los productos deben mostrarse agrupados por nombre nombre de producto.</t>
+  </si>
+  <si>
+    <t>Fallo</t>
+  </si>
+  <si>
+    <t>No se observan validaciones ni mensajes de alerta por parte del sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema no notifica si hay datos faltantes o si el pedido se registró con éxito por lo cual deja con incertidumbre al usuario acerca del estado del mismo. </t>
+  </si>
+  <si>
+    <t>Severo</t>
+  </si>
+  <si>
+    <t>Creado</t>
+  </si>
+  <si>
+    <t>Pasos para reproducirlo</t>
+  </si>
+  <si>
+    <t>Al ingresar un valor para el campo de "Dirección", éste no es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que el mismo quede vacío, notificando de la situación.</t>
+  </si>
+  <si>
+    <t>1. Ingresar un valor alfanumérico (para nombre y para el número de la dirección asociado) al campo "Dirección".
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar el campo "Dirección". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar el campo "Ciudad". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>Al seleccionar un valor para el campo de "Ciudad", éste no es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que el mismo quede vacío, notificando de la situación.</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar el campo "Referencia Opcional". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>Al ingresar un valor para el campo de "Referencia Opcional", éste no es validado por el sistema.</t>
+  </si>
+  <si>
+    <t>1. Ingresar texto en el campo "Referencia Opcional".
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>Menor</t>
+  </si>
+  <si>
+    <t>Al seleccionar el valor "Efectivo" para el campo de "Forma de Pago", éste no es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que el mismo quede vacío, notificando de la situación.</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar el campo "Monto" al haber seleccionado la opción "Efectivo" para la Forma de Pago elegida. Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>1. Seleccionar un valor del menú desplegable de Ciudades.
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Efectivo" del menú desplegable de "Forma de Pago".
+2. Ingresar un monto en el campo de "Monto".
+3. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la forma de pago "Efectivo".
+2. El usuario ingresa el monto a pagar "400".
+3. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+2. El sistema valida que el usuario haya ingresado un monto válido para el pago, comprobando que "400" sea un número válido (mayor o igual al monto a pagar ("450")), y lo es.
+3. El sistema muestra el mensaje "¡El monto ingresado es insuficiente! Coloque un monto válido".</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar los campos "Número de Tarjeta", ni "Nombre", ni "Apellido", ni "Fecha de Vencimiento", ni "CVC" al haber seleccionado la opción "Pago con Tarjeta VISA" para la Forma de Pago elegida. Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
+2. Ingresar un número de tarjeta.
+3. Ingresar el nombre del titular de la tarjeta ingresada.
+4. Ingresar el apellido del titular de la tarjeta ingresada.
+5. Ingresar la fecha de vencimiento de la tarjeta ingresada.
+6. Ingresar el código CVC de la tarjeta ingresada.
+7. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar el campo de "Momento de Entrega" al haber seleccionado la opción "Lo Antes Posible". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Lo Antes Posible" para el momento de entrega.
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar los campos de "Fecha de Entrega" y "Hora de Entrega" al haber seleccionado la opción "Fecha y Hora de Recepción". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>Al seleccionar la opción "Lo Antes Posible" para el momento de entrega del pedido, y confirmar el mismo, el sistema no hace nada, ni genera ningún tipo de notificación.</t>
+  </si>
+  <si>
+    <t>1. Ingresar un valor válido para la fecha deseada para la recepción del pedido.
+2. Ingresar un valor válido para la hora deseada para la recepción del pedido.
+3. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>Los productos iguales no se muestran agrupados.</t>
+  </si>
+  <si>
+    <t>Al seleccionar la opción "Ver Pedido", una vez que se hayan agregado productos al carrito, éstos no se muestran agrupados en caso de ser iguales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar la opción "Ver Pedido".
 </t>
   </si>
   <si>
-    <t>Fecha y Hora Estimada de Llegada</t>
-  </si>
-  <si>
-    <t>Visualización de la fecha y hora estimada de la llegada del pedido.</t>
-  </si>
-  <si>
-    <t>El usuario tiene que estar logueado con el Rol de "Comprador", tiene que haber seleccionado uno o más productos para que se hayan agregado al carrito de compras, y tiene que tener un pedido realizado.</t>
-  </si>
-  <si>
-    <t>El usuario tiene que estar logueado con el Rol de "Comprador", y tiene que haber seleccionado uno o más productos para que se hayan agregado al carrito de compras.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la opción "Ver mis pedidos".</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla del pedido con los productos del mismo, el monto total, la forma de pago elegida, y la fecha y hora estimada de llegada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema muestra la pantalla del carrito con los productos que se hayan agregado. Los productos iguales no se muestran agrupados. </t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla del carrito con los productos que se hayan agregado. Los productos deben mostrarse agrupados por nombre nombre de producto.</t>
-  </si>
-  <si>
-    <t>Fallo</t>
-  </si>
-  <si>
-    <t>Los productos iguales no se muestran agrupados</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la opción "Ver mis pedidos"</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona la opción "Ver mis pedidos".
-2. El usuario selecciona la opción 'editar' de un detalle del pedido.</t>
-  </si>
-  <si>
-    <t>Editar detalle de pedido</t>
-  </si>
-  <si>
-    <t>No se observan validaciones ni mensajes de alerta por parte del sistema.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema no notifica si hay datos faltantes o si el pedido se registró con éxito por lo cual deja con incertidumbre al usuario acerca del estado del mismo. </t>
-  </si>
-  <si>
-    <t>Funcionalidad inaccesible</t>
-  </si>
-  <si>
-    <t>No es posible registrar un pedido exitosamente</t>
-  </si>
-  <si>
-    <t>Severo</t>
-  </si>
-  <si>
-    <t>Creado</t>
-  </si>
-  <si>
-    <t>Pasos para reproducirlo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema no aparenta validar los campos de dirección </t>
+    <t xml:space="preserve">1. El usuario selecciona la opción de "Ver Pedido".
+</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Ver Pedido".</t>
+  </si>
+  <si>
+    <t>Funcionalidad inaccesible.</t>
+  </si>
+  <si>
+    <t>No es posible registrar un pedido exitosamente.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Ver Pedido".
+2. El usuario selecciona la opción "Editar" de un detalle del pedido.</t>
+  </si>
+  <si>
+    <t>1. El sistema actualiza el detalle de pedido de acuerdo a si se modificó la cantidad del producto solicitado, o si se eliminó un producto del detalle, y lo muestra.</t>
+  </si>
+  <si>
+    <t>No es posible confirmar un pedido una vez que ya se han agregado productos al carrito, e ingresado los datos requeridos (dirección, ciudad, etc.), por lo que no es posible ver la fecha y hora estimada de llegada del pedido. A su vez, tampoco es posible modificar la cantidad de un producto que ya esté en el carrito, o quitarlo del mismo.</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Ver Pedido".
+2. Seleccionar el producto que se desea modificar, o eliminar, cambiando el número de productos, o eliminándolo en caso de querer retirarlo del detalle de pedido.</t>
+  </si>
+  <si>
+    <t>Realización del pedido.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario tiene que haber seleccionado previamente algún producto del comercio adherido, y haberlo agregado al carrito.
+</t>
+  </si>
+  <si>
+    <t>Al ingresar un valor para los campos "Número de Tarjeta", "Nombre", "Apellido", "Fecha de Vencimiento" y "CVC", ninguno es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que alguno de estos campos queden vacíos, notificando de la situación.</t>
+  </si>
+  <si>
+    <t>Editar detalle de pedido.</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el nombre de calle "598" sea solo texto, y que sea un nombre válido, y no lo es.
+2. El sistema valida que el usuario haya seleccionado una opción del menú desplegable, que la opción " " sea inválida, y no es así.
+3. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
+4. El sistema valida que la fecha ingresada por el usuario "15/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y es así.
+5. El sistema valida que la hora ingresada por el usuario "22:00" sea una hora con formato válido, mayor a la hora actual, y es así.
+6. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+7. El sistema valida que el número de tarjeta ingresado por el usuario "0000 1111 2222 3333" sea un número de tarjeta inválido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
+8. El sistema valida que el nombre y apellido "156" sea texto válido, y no lo es.
+9. El sistema valida que la fecha de vencimiento "04/17" sea válida, y no lo es.
+10. El sistema valida que el código CVC "0" ingresado sea inválido, y no lo es.
+11. El sistema muestra el mensaje "Datos erróneos".</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar los campos "Dirección", ni "Ciudad", ni "Fecha Deseada", ni "Hora Deseada", ni "Número de Tarjeta", ni "Nombre", ni "Apellido", ni "Fecha de Vencimiento" ni "CVC". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>Al seleccionar la opción "Fecha y Hora de Recepción" para el momento de entrega del pedido, ingresar valores válidos para los campos "Fecha Deseada" y "Hora Deseada", y confirmar el mismo, el sistema no hace nada, ni genera ningún tipo de notificación.</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresa el nombre de calle "598".
+2. El usuario no selecciona valor para el campo "Ciudad" del menú desplegable.
+3. El usuario selecciona la opción "Determinar fecha y hora de recepción".
+4. El usuario ingresa la fecha "15/09/2019" como fecha de recepción.
+5. El usuario ingresa la hora "25:00" como hora de recepción.
+6. El usuario selecciona la forma de pago "Tarjeta VISA".
+7. El usuario ingresa el número de tarjeta "0000 1111 2222 3333".
+8. El usuario ingresa nombre y apellido "156".
+9. El usuario ingresa fecha de vencimiento de la tarjeta "04/17".
+10. El usuario ingresa el CVC "0". 
+11. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. Ingresar un valor numérico para el campo "Dirección".
+2. No seleccionar ninguna opción para el campo "Ciudad" del menú desplegable de Ciudades.
+3. Seleccionar la opción "Determinar fecha y hora de recepción".
+4. Ingresar una fecha inválida como fecha de recepción (por ejemplo, anterior a la fecha actual).
+5. Ingresar una hora de recepción.
+6. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
+7. Ingresar un número inválido de tarjeta (por ejemplo, que comienza con '0000').
+8. Ingresar un valor numérico como nombre del titular de la tarjeta.
+9. Ingresar un valor numérico como apellido del titular de la tarjeta.
+10. Ingresar una fecha anterior a la fecha actual como fecha de vencimiento de la tarjeta.
+11. Ingresar un código CVC inválido (por ejemplo, '0').
+12. Seleccionar la opción "Aceptar".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -687,8 +727,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,6 +785,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,7 +1005,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1081,20 +1132,86 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="DataPilot Category" xfId="1"/>
-    <cellStyle name="DataPilot Corner" xfId="2"/>
-    <cellStyle name="DataPilot Field" xfId="3"/>
-    <cellStyle name="DataPilot Result" xfId="4"/>
-    <cellStyle name="DataPilot Title" xfId="5"/>
-    <cellStyle name="DataPilot Value" xfId="6"/>
+    <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="DataPilot Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="DataPilot Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="DataPilot Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="DataPilot Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="DataPilot Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="240">
+  <dxfs count="130">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1156,55 +1273,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1229,69 +1297,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1316,55 +1321,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1438,6 +1394,55 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1462,55 +1467,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1535,55 +1491,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1608,55 +1515,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="51"/>
           <bgColor indexed="13"/>
@@ -1682,20 +1540,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
@@ -1842,6 +1686,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
@@ -1998,54 +1856,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -2095,30 +1905,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -2163,541 +1949,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3279,15 +2530,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS71"/>
+  <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3351,7 +2602,7 @@
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -3452,7 +2703,7 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="47" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="43"/>
@@ -3520,21 +2771,21 @@
       <c r="F8" s="48"/>
       <c r="G8" s="48"/>
       <c r="H8" s="46" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I8" s="46"/>
       <c r="J8" s="46"/>
       <c r="K8" s="46"/>
       <c r="L8" s="46"/>
       <c r="M8" s="46" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="N8" s="46"/>
       <c r="O8" s="46"/>
       <c r="P8" s="46"/>
       <c r="Q8" s="46"/>
       <c r="R8" s="46" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="S8" s="46"/>
       <c r="T8" s="46"/>
@@ -3543,70 +2794,70 @@
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="K9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>75</v>
-      </c>
       <c r="M9" s="14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="P9" s="25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R9" s="14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="U9" s="25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="V9" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AB9" s="3"/>
       <c r="AL9" s="3"/>
@@ -3637,39 +2888,39 @@
       <c r="AB10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="108" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="K11" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="37">
         <v>43753</v>
@@ -3691,36 +2942,36 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="108" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="K12" s="29">
         <v>2</v>
@@ -3745,39 +2996,39 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="108" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E13" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>103</v>
-      </c>
       <c r="G13" s="26" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="K13" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L13" s="37">
         <v>43753</v>
@@ -3799,39 +3050,39 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="K14" s="29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L14" s="37">
         <v>43753</v>
@@ -3853,39 +3104,39 @@
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
     </row>
-    <row r="15" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="E15" s="26" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="K15" s="29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L15" s="37">
         <v>43753</v>
@@ -3907,39 +3158,39 @@
       <c r="AR15" s="7"/>
       <c r="AS15" s="7"/>
     </row>
-    <row r="16" spans="1:45" ht="180" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="K16" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L16" s="37">
         <v>43753</v>
@@ -3961,39 +3212,39 @@
       <c r="AR16" s="7"/>
       <c r="AS16" s="7"/>
     </row>
-    <row r="17" spans="1:45" ht="120" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" ht="156" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C17" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="21" t="s">
-        <v>129</v>
-      </c>
       <c r="E17" s="26" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="K17" s="29">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L17" s="37">
         <v>43753</v>
@@ -4015,39 +3266,39 @@
       <c r="AR17" s="7"/>
       <c r="AS17" s="7"/>
     </row>
-    <row r="18" spans="1:45" ht="84" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>111</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="K18" s="29">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L18" s="37">
         <v>43753</v>
@@ -4069,42 +3320,42 @@
       <c r="AR18" s="7"/>
       <c r="AS18" s="7"/>
     </row>
-    <row r="19" spans="1:45" ht="120" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F19" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="26" t="s">
-        <v>119</v>
-      </c>
       <c r="H19" s="26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J19" s="28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K19" s="29">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L19" s="37">
-        <v>43753</v>
+        <v>43753.45208333333</v>
       </c>
       <c r="M19" s="39"/>
       <c r="N19" s="15"/>
@@ -4123,39 +3374,39 @@
       <c r="AR19" s="7"/>
       <c r="AS19" s="7"/>
     </row>
-    <row r="20" spans="1:45" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" ht="72" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>111</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J20" s="28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K20" s="29">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L20" s="37">
         <v>43753</v>
@@ -4177,42 +3428,42 @@
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
     </row>
-    <row r="21" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" ht="312" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>137</v>
+        <v>44</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>159</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="K21" s="29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L21" s="37">
-        <v>43753.45208333333</v>
+        <v>43753</v>
       </c>
       <c r="M21" s="39"/>
       <c r="N21" s="15"/>
@@ -4231,43 +3482,20 @@
       <c r="AR21" s="7"/>
       <c r="AS21" s="7"/>
     </row>
-    <row r="22" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="K22" s="29">
-        <v>3</v>
-      </c>
-      <c r="L22" s="37">
-        <v>43753</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="37"/>
       <c r="M22" s="39"/>
       <c r="N22" s="15"/>
       <c r="O22" s="28"/>
@@ -4285,43 +3513,21 @@
       <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
     </row>
-    <row r="23" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="K23" s="29">
-        <v>3</v>
-      </c>
-      <c r="L23" s="37">
-        <v>43753</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="37"/>
       <c r="M23" s="39"/>
       <c r="N23" s="15"/>
       <c r="O23" s="28"/>
@@ -4339,25 +3545,15 @@
       <c r="AR23" s="7"/>
       <c r="AS23" s="7"/>
     </row>
-    <row r="24" spans="1:45" ht="72" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>150</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
       <c r="I24" s="15"/>
@@ -4383,7 +3579,7 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -4415,7 +3611,7 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -4447,7 +3643,7 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -4479,7 +3675,7 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -4511,7 +3707,7 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -4543,7 +3739,7 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -4575,7 +3771,7 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -4607,7 +3803,7 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -4639,7 +3835,7 @@
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -4671,7 +3867,7 @@
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -5636,8 +4832,8 @@
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
       <c r="D64" s="21"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
       <c r="G64" s="26"/>
       <c r="H64" s="26"/>
       <c r="I64" s="15"/>
@@ -5668,8 +4864,8 @@
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
       <c r="G65" s="26"/>
       <c r="H65" s="26"/>
       <c r="I65" s="15"/>
@@ -5732,8 +4928,8 @@
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
       <c r="G67" s="26"/>
       <c r="H67" s="26"/>
       <c r="I67" s="15"/>
@@ -5762,10 +4958,10 @@
         <v>34</v>
       </c>
       <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
       <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
+      <c r="F68" s="26"/>
       <c r="G68" s="26"/>
       <c r="H68" s="26"/>
       <c r="I68" s="15"/>
@@ -5789,104 +4985,8 @@
       <c r="AR68" s="7"/>
       <c r="AS68" s="7"/>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A69" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="29"/>
-      <c r="L69" s="37"/>
-      <c r="M69" s="39"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="28"/>
-      <c r="P69" s="29"/>
-      <c r="Q69" s="16"/>
-      <c r="R69" s="39"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="28"/>
-      <c r="U69" s="29"/>
-      <c r="V69" s="16"/>
-      <c r="AN69" s="7"/>
-      <c r="AO69" s="7"/>
-      <c r="AP69" s="7"/>
-      <c r="AQ69" s="7"/>
-      <c r="AR69" s="7"/>
-      <c r="AS69" s="7"/>
-    </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A70" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="26"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="28"/>
-      <c r="K70" s="29"/>
-      <c r="L70" s="37"/>
-      <c r="M70" s="39"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="28"/>
-      <c r="P70" s="29"/>
-      <c r="Q70" s="16"/>
-      <c r="R70" s="39"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="28"/>
-      <c r="U70" s="29"/>
-      <c r="V70" s="16"/>
-      <c r="AN70" s="7"/>
-      <c r="AO70" s="7"/>
-      <c r="AP70" s="7"/>
-      <c r="AQ70" s="7"/>
-      <c r="AR70" s="7"/>
-      <c r="AS70" s="7"/>
-    </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A71" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="28"/>
-      <c r="K71" s="29"/>
-      <c r="L71" s="37"/>
-      <c r="M71" s="39"/>
-      <c r="N71" s="15"/>
-      <c r="O71" s="28"/>
-      <c r="P71" s="29"/>
-      <c r="Q71" s="16"/>
-      <c r="R71" s="39"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="28"/>
-      <c r="U71" s="29"/>
-      <c r="V71" s="16"/>
-      <c r="AN71" s="7"/>
-      <c r="AO71" s="7"/>
-      <c r="AP71" s="7"/>
-      <c r="AQ71" s="7"/>
-      <c r="AR71" s="7"/>
-      <c r="AS71" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A9:AS2329"/>
+  <autoFilter ref="A9:AS2326" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A2:F4"/>
     <mergeCell ref="H8:L8"/>
@@ -5896,419 +4996,431 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="D5:F5"/>
   </mergeCells>
-  <conditionalFormatting sqref="J621:J745 J747 J749 J751 J753 J755 J757 J759 J761 J763:J769 J917:J1040 J1042:J1179 J1184:J1198 J1203:J1207 J1212:J1261 J1265:J1289 J1291:J1383 J1387:J1411 J1413:J1472 J1474:J1560 J1599:J1620 J1757:J1758 J1761:J1788 J1916:J1957 J1960:J1962 J1965 J1967:J1969 J1972:J2009 J2012:J2052 J2055:J2077 J2080:J2083 J2086 J2088:J2090 J2093:J2134 J2330:J65042 O621:O745 O747 O749 O751 O753 O755 O757 O759 O761 O763:O769 O917:O1040 O1042:O1179 O1184:O1198 O1203:O1207 O1212:O1261 O1265:O1289 O1291:O1383 O1387:O1411 O1413:O1472 O1474:O1560 O1599:O1620 O1757:O1758 O1761:O1788 O1916:O1957 O1960:O1962 O1965 O1967:O1969 O1972:O2009 O2012:O2052 O2055:O2077 O2080:O2083 O2086 O2088:O2090 O2093:O2134 O2330:O65042 J21:J22 J24:J604 O9:O604 J9:J11 T11:T604">
-    <cfRule type="cellIs" dxfId="139" priority="168" stopIfTrue="1" operator="equal">
+  <phoneticPr fontId="17" type="noConversion"/>
+  <conditionalFormatting sqref="J618:J742 J744 J746 J748 J750 J752 J754 J756 J758 J760:J766 J914:J1037 J1039:J1176 J1181:J1195 J1200:J1204 J1209:J1258 J1262:J1286 J1288:J1380 J1384:J1408 J1410:J1469 J1471:J1557 J1596:J1617 J1754:J1755 J1758:J1785 J1913:J1954 J1957:J1959 J1962 J1964:J1966 J1969:J2006 J2009:J2049 J2052:J2074 J2077:J2080 J2083 J2085:J2087 J2090:J2131 J2327:J65039 O618:O742 O744 O746 O748 O750 O752 O754 O756 O758 O760:O766 O914:O1037 O1039:O1176 O1181:O1195 O1200:O1204 O1209:O1258 O1262:O1286 O1288:O1380 O1384:O1408 O1410:O1469 O1471:O1557 O1596:O1617 O1754:O1755 O1758:O1785 O1913:O1954 O1957:O1959 O1962 O1964:O1966 O1969:O2006 O2009:O2049 O2052:O2074 O2077:O2080 O2083 O2085:O2087 O2090:O2131 O2327:O65039 J9:J11 J23:J601 O9:O601 T11:T601 J18:J21">
+    <cfRule type="cellIs" dxfId="129" priority="238" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="169" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="239" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="170" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="240" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I22 I24:I71 I11 N11:N71 S11:S71">
-    <cfRule type="cellIs" dxfId="136" priority="160" operator="equal">
+  <conditionalFormatting sqref="I11 I23:I68 N11:N68 S11:S68 I18:I21">
+    <cfRule type="cellIs" dxfId="126" priority="230" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="231" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="232" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="233" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="234" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I22 I24:I71 I11 N11:N71 S11:S71">
-    <cfRule type="cellIs" dxfId="131" priority="145" operator="equal">
+  <conditionalFormatting sqref="I11 I23:I68 N11:N68 S11:S68 I18:I21">
+    <cfRule type="cellIs" dxfId="121" priority="215" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="216" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T621:T745 T747 T749 T751 T753 T755 T757 T759 T761 T763:T769 T917:T1040 T1042:T1179 T1184:T1198 T1203:T1207 T1212:T1261 T1265:T1289 T1291:T1383 T1387:T1411 T1413:T1472 T1474:T1560 T1599:T1620 T1757:T1758 T1761:T1788 T1916:T1957 T1960:T1962 T1965 T1967:T1969 T1972:T2009 T2012:T2052 T2055:T2077 T2080:T2083 T2086 T2088:T2090 T2093:T2134 T2330:T65042 T9:T10">
-    <cfRule type="cellIs" dxfId="129" priority="135" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="T618:T742 T744 T746 T748 T750 T752 T754 T756 T758 T760:T766 T914:T1037 T1039:T1176 T1181:T1195 T1200:T1204 T1209:T1258 T1262:T1286 T1288:T1380 T1384:T1408 T1410:T1469 T1471:T1557 T1596:T1617 T1754:T1755 T1758:T1785 T1913:T1954 T1957:T1959 T1962 T1964:T1966 T1969:T2006 T2009:T2049 T2052:T2074 T2077:T2080 T2083 T2085:T2087 T2090:T2131 T2327:T65039 T9:T10">
+    <cfRule type="cellIs" dxfId="119" priority="205" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="136" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="206" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="137" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="207" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="116" priority="163" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="164" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="165" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="166" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="167" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="111" priority="161" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="162" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="109" priority="153" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="154" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="155" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="156" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="157" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="104" priority="151" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="152" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="102" priority="143" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="144" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="145" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="146" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="147" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="97" priority="141" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="142" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="95" priority="123" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="124" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="125" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="126" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="127" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="90" priority="121" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="122" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
+    <cfRule type="cellIs" dxfId="88" priority="118" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="119" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="120" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" dxfId="85" priority="113" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="114" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="115" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="116" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="117" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" dxfId="80" priority="111" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="112" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="78" priority="103" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="104" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="105" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="106" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="107" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="73" priority="101" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="102" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="cellIs" dxfId="69" priority="88" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="89" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="90" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="66" priority="83" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="84" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="85" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="86" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="87" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="61" priority="81" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="82" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20">
+    <cfRule type="cellIs" dxfId="59" priority="78" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="79" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="80" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="56" priority="73" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="74" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="75" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="76" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="77" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="99" priority="98" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="68" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="99" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="69" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="100" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="70" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="96" priority="93" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="94" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="96" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
-      <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="89" priority="88" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="62" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="89" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="63" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="90" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="64" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="86" priority="83" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="84" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="86" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="87" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
-      <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="79" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="79" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="57" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="80" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="76" priority="73" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="74" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="76" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="77" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
-      <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="69" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="54" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="55" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="66" priority="63" operator="equal">
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="49" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="37" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="cellIs" dxfId="59" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="54" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="57" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
-      <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="cellIs" dxfId="49" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
+  <conditionalFormatting sqref="J22">
+    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="39" priority="38" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="cellIs" dxfId="29" priority="28" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" stopIfTrue="1" operator="equal">
-      <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
-    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
-      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P65:P66 K65:K66 U65:U66"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N11:N71 S11:S71 I11:I71">
+    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P62:P63 K62:K63 U62:U63" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I23:I68 S11:S68 N11:N68 I11:I21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B15:B71">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B23:B68 B15:B21" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6319,11 +5431,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6347,28 +5459,28 @@
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -6381,151 +5493,265 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="21" t="s">
+        <v>0</v>
+      </c>
       <c r="C4" s="44">
         <v>43753</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="26"/>
+      <c r="D4" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>127</v>
+      </c>
       <c r="F4" s="21" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="C5" s="44">
         <v>43753</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="D5" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="H5" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="C6" s="44">
         <v>43753</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="D6" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>109</v>
+      </c>
       <c r="H6" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="C7" s="44">
         <v>43753</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="132" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>5</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>38</v>
+      </c>
       <c r="C8" s="44">
         <v>43753</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>6</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="44">
         <v>43753</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>7</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" s="44">
         <v>43753</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>8</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="C11" s="44">
         <v>43753</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D11" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>9</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="44">
+        <v>43753</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="252" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>10</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="B13" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="44">
+        <v>43753</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
@@ -6533,8 +5759,8 @@
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
@@ -6545,8 +5771,8 @@
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
@@ -6557,8 +5783,8 @@
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -6569,8 +5795,8 @@
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -6581,21 +5807,21 @@
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6604,12 +5830,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6739,17 +5964,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6773,11 +6001,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificaciones en el excel de casos de prueba
</commit_message>
<xml_diff>
--- a/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
+++ b/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Archivos Generales\Facultad\ISW\Repositorio\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043D7090-8883-4E8A-93B4-976CB209ED81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A510E4-87A2-492C-875C-E72D43FAA5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,15 +293,6 @@
 3. El sistema valida que el número de calle "430" sea numérico y válido, y lo es.</t>
   </si>
   <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Validación de la ciudad seleccionada para pedido.</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el usuario haya seleccionado una opción del menú desplegable, que la opción "Córdoba" sea válida, y es así.</t>
-  </si>
-  <si>
     <t>Media</t>
   </si>
   <si>
@@ -309,18 +300,10 @@
   </si>
   <si>
     <t>Validación de la referencia opcional ingresada para pedido.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona como opción del menú desplegable de ciudades, la opción "Córdoba".
-2. El usuario continúa con el ingreso de los demás datos.</t>
   </si>
   <si>
     <t>1. El usuario ingresa como referencia opcional "Edificio con puerta de vidrio ubicado entre un kiosco y una panadería".
 2. El usuario continúa con el ingreso de los demás datos.</t>
-  </si>
-  <si>
-    <t>1. El sistema valida si el usuario ingresó o no algo en el campo de "Referencia Opcional".
-2. El sistema valida que el texto ingresado "Edificio con puerta de vicrio ubicado entre un kiosco y una panadería" sea un texto alfanumérico, o solo texto válido, y lo es.</t>
   </si>
   <si>
     <t>Forma de Pago</t>
@@ -446,9 +429,6 @@
     <t>El sistema no aparenta validar el campo "Dirección". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
   </si>
   <si>
-    <t>El sistema no aparenta validar el campo "Ciudad". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
-  </si>
-  <si>
     <t>Al seleccionar un valor para el campo de "Ciudad", éste no es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que el mismo quede vacío, notificando de la situación.</t>
   </si>
   <si>
@@ -493,15 +473,6 @@
     <t>El sistema no aparenta validar los campos "Número de Tarjeta", ni "Nombre", ni "Apellido", ni "Fecha de Vencimiento", ni "CVC" al haber seleccionado la opción "Pago con Tarjeta VISA" para la Forma de Pago elegida. Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
   </si>
   <si>
-    <t>1. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
-2. Ingresar un número de tarjeta.
-3. Ingresar el nombre del titular de la tarjeta ingresada.
-4. Ingresar el apellido del titular de la tarjeta ingresada.
-5. Ingresar la fecha de vencimiento de la tarjeta ingresada.
-6. Ingresar el código CVC de la tarjeta ingresada.
-7. Hacer clic en el botón de "Confirmar Pedido".</t>
-  </si>
-  <si>
     <t>El sistema no aparenta validar el campo de "Momento de Entrega" al haber seleccionado la opción "Lo Antes Posible". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
   </si>
   <si>
@@ -564,56 +535,94 @@
 </t>
   </si>
   <si>
-    <t>Al ingresar un valor para los campos "Número de Tarjeta", "Nombre", "Apellido", "Fecha de Vencimiento" y "CVC", ninguno es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que alguno de estos campos queden vacíos, notificando de la situación.</t>
-  </si>
-  <si>
     <t>Editar detalle de pedido.</t>
   </si>
   <si>
+    <t>Al seleccionar la opción "Fecha y Hora de Recepción" para el momento de entrega del pedido, ingresar valores válidos para los campos "Fecha Deseada" y "Hora Deseada", y confirmar el mismo, el sistema no hace nada, ni genera ningún tipo de notificación.</t>
+  </si>
+  <si>
+    <t>Ciudad, Provincia y Código Postal</t>
+  </si>
+  <si>
+    <t>Validación de la ciudad, provincia y código postal ingresados.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona como opción del menú desplegable de ciudades, la opción "Córdoba".
+2. El usuario selecciona como opción del menú desplegable de provincias, la opción "Córdoba".
+3. El usuario ingresa el código postal "5000".
+4. El usuario continúa con el ingreso de los demás datos.</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar los campos "Ciudad", ni "Provincia", ni "ZIP". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de ciudades, que la opción "Córdoba" sea válida, y es así.
+2. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de provincias, que la opción "Córdoba" sea válida, y es así.
+3. El sistema valida que el usuario haya intresado un valor numérico para el campo "ZIP".</t>
+  </si>
+  <si>
+    <t>1. El sistema valida si el usuario ingresó o no algo en el campo de "Referencia Opcional".
+2. El sistema valida que el texto ingresado "Edificio con puerta de vidrio ubicado entre un kiosco y una panadería" sea un texto alfanumérico, o solo texto válido, y lo es.</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresa el nombre de calle "598".
+2. El usuario no selecciona valor para el campo "Ciudad" del menú desplegable de Ciudad.
+3. El usuario no selecciona valor para el campo "Provincia" del menú desplegable de Provincia.
+4. El usuario ingresa el valor "aaa" para el campo "ZIP".
+5. El usuario selecciona la opción "Determinar fecha y hora de recepción".
+6. El usuario ingresa la fecha "15/09/2019" como fecha de recepción.
+7. El usuario ingresa la hora "25:00" como hora de recepción.
+8. El usuario selecciona la forma de pago "Tarjeta VISA".
+9. El usuario ingresa el número de tarjeta "0000 1111 2222 3333".
+10. El usuario ingresa nombre y apellido "156".
+11. El usuario ingresa fecha de vencimiento de la tarjeta "04/17".
+12. El usuario ingresa el CVC "0". 
+13. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
     <t>1. El sistema valida que el nombre de calle "598" sea solo texto, y que sea un nombre válido, y no lo es.
-2. El sistema valida que el usuario haya seleccionado una opción del menú desplegable, que la opción " " sea inválida, y no es así.
-3. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
-4. El sistema valida que la fecha ingresada por el usuario "15/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y es así.
-5. El sistema valida que la hora ingresada por el usuario "22:00" sea una hora con formato válido, mayor a la hora actual, y es así.
-6. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-7. El sistema valida que el número de tarjeta ingresado por el usuario "0000 1111 2222 3333" sea un número de tarjeta inválido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
-8. El sistema valida que el nombre y apellido "156" sea texto válido, y no lo es.
-9. El sistema valida que la fecha de vencimiento "04/17" sea válida, y no lo es.
+2. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de Ciudad, que la opción " " sea inválida, y no es así.
+3. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de Pronvincia, que la opción " " sea inválida, y no es así.
+4. El sistema valida que el valor de código postal ingresado "aaa" sea numérico, válido, y no lo es.
+5. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
+6. El sistema valida que la fecha ingresada por el usuario "15/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y es así.
+7. El sistema valida que la hora ingresada por el usuario "22:00" sea una hora con formato válido, mayor a la hora actual, y es así.
+8. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+9. El sistema valida que el número de tarjeta ingresado por el usuario "0000 1111 2222 3333" sea un número de tarjeta inválido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
+10. El sistema valida que el nombre y apellido "156" sea texto válido, y no lo es.
+11. El sistema valida que la fecha de vencimiento "04/17" sea válida, y no lo es.
 10. El sistema valida que el código CVC "0" ingresado sea inválido, y no lo es.
-11. El sistema muestra el mensaje "Datos erróneos".</t>
-  </si>
-  <si>
-    <t>El sistema no aparenta validar los campos "Dirección", ni "Ciudad", ni "Fecha Deseada", ni "Hora Deseada", ni "Número de Tarjeta", ni "Nombre", ni "Apellido", ni "Fecha de Vencimiento" ni "CVC". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
-  </si>
-  <si>
-    <t>Al seleccionar la opción "Fecha y Hora de Recepción" para el momento de entrega del pedido, ingresar valores válidos para los campos "Fecha Deseada" y "Hora Deseada", y confirmar el mismo, el sistema no hace nada, ni genera ningún tipo de notificación.</t>
-  </si>
-  <si>
-    <t>1. El usuario ingresa el nombre de calle "598".
-2. El usuario no selecciona valor para el campo "Ciudad" del menú desplegable.
-3. El usuario selecciona la opción "Determinar fecha y hora de recepción".
-4. El usuario ingresa la fecha "15/09/2019" como fecha de recepción.
-5. El usuario ingresa la hora "25:00" como hora de recepción.
-6. El usuario selecciona la forma de pago "Tarjeta VISA".
-7. El usuario ingresa el número de tarjeta "0000 1111 2222 3333".
-8. El usuario ingresa nombre y apellido "156".
-9. El usuario ingresa fecha de vencimiento de la tarjeta "04/17".
-10. El usuario ingresa el CVC "0". 
-11. El usuario selecciona la opción "Aceptar".</t>
+13. El sistema muestra el mensaje "Datos erróneos".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
+2. Ingresar un número de tarjeta.
+3. Ingresar el nombre y apellido del titular de la tarjeta ingresada.
+4. Ingresar la fecha de vencimiento de la tarjeta ingresada.
+5. Ingresar el código CVC de la tarjeta ingresada.
+6. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>Al ingresar un valor para los campos "Número de Tarjeta", "Nombre y Apellido", "Fecha de Vencimiento" y "CVC", ninguno es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que alguno de estos campos queden vacíos, notificando de la situación.</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar los campos "Dirección", ni "Ciudad", ni "Fecha Deseada", ni "Hora Deseada", ni "Número de Tarjeta", ni "Nombre y Apellido", ni "Fecha de Vencimiento" ni "CVC". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
   </si>
   <si>
     <t>1. Ingresar un valor numérico para el campo "Dirección".
 2. No seleccionar ninguna opción para el campo "Ciudad" del menú desplegable de Ciudades.
-3. Seleccionar la opción "Determinar fecha y hora de recepción".
-4. Ingresar una fecha inválida como fecha de recepción (por ejemplo, anterior a la fecha actual).
-5. Ingresar una hora de recepción.
-6. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
-7. Ingresar un número inválido de tarjeta (por ejemplo, que comienza con '0000').
-8. Ingresar un valor numérico como nombre del titular de la tarjeta.
-9. Ingresar un valor numérico como apellido del titular de la tarjeta.
-10. Ingresar una fecha anterior a la fecha actual como fecha de vencimiento de la tarjeta.
-11. Ingresar un código CVC inválido (por ejemplo, '0').
-12. Seleccionar la opción "Aceptar".</t>
+3. No seleccionar ninguna opción para el campo "Provincia" del menú desplegable de Provincias.
+4. Ingresar un valor de texto para el campo "ZIP".
+5. Seleccionar la opción "Determinar fecha y hora de recepción".
+6. Ingresar una fecha inválida como fecha de recepción (por ejemplo, anterior a la fecha actual).
+7. Ingresar una hora de recepción.
+8. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
+9. Ingresar un número inválido de tarjeta (por ejemplo, que comienza con '0000').
+10. Ingresar un valor numérico como nombre del titular de la tarjeta.
+11. Ingresar un valor numérico como apellido del titular de la tarjeta.
+12. Ingresar una fecha anterior a la fecha actual como fecha de vencimiento de la tarjeta.
+13. Ingresar un código CVC inválido (por ejemplo, '0').
+14. Seleccionar la opción "Aceptar".</t>
   </si>
 </sst>
 </file>
@@ -1111,6 +1120,9 @@
     <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1132,9 +1144,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1148,105 +1157,7 @@
     <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="130">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="116">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2536,9 +2447,9 @@
   </sheetPr>
   <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2601,14 +2512,14 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
       <c r="I2" s="32"/>
@@ -2636,12 +2547,12 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -2669,12 +2580,12 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -2702,14 +2613,14 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="43"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -2763,34 +2674,34 @@
     </row>
     <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="46" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46" t="s">
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46" t="s">
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -2893,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>81</v>
@@ -2911,13 +2822,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K11" s="29">
         <v>1</v>
@@ -2942,36 +2853,36 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="108" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="120" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>83</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="K12" s="29">
         <v>2</v>
@@ -3001,31 +2912,31 @@
         <v>36</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>83</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K13" s="29">
         <v>3</v>
@@ -3058,28 +2969,28 @@
         <v>80</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="K14" s="29">
         <v>4</v>
@@ -3112,28 +3023,28 @@
         <v>80</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K15" s="29">
         <v>5</v>
@@ -3166,28 +3077,28 @@
         <v>80</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="K16" s="29">
         <v>6</v>
@@ -3220,28 +3131,28 @@
         <v>80</v>
       </c>
       <c r="C17" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="E17" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>106</v>
-      </c>
       <c r="G17" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K17" s="29">
         <v>7</v>
@@ -3274,28 +3185,28 @@
         <v>80</v>
       </c>
       <c r="C18" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>116</v>
-      </c>
       <c r="F18" s="26" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K18" s="29">
         <v>8</v>
@@ -3325,31 +3236,31 @@
         <v>42</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E19" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>120</v>
-      </c>
       <c r="J19" s="28" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="K19" s="29">
         <v>9</v>
@@ -3379,31 +3290,31 @@
         <v>43</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I20" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F20" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>120</v>
-      </c>
       <c r="J20" s="28" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="K20" s="29">
         <v>9</v>
@@ -3428,36 +3339,36 @@
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
     </row>
-    <row r="21" spans="1:45" ht="312" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" ht="372" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="52" t="s">
-        <v>159</v>
+      <c r="C21" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>152</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G21" s="26" t="s">
         <v>163</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K21" s="29">
         <v>10</v>
@@ -3486,13 +3397,13 @@
       <c r="A22" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
       <c r="J22" s="28"/>
       <c r="K22" s="29"/>
       <c r="L22" s="37"/>
@@ -4998,420 +4909,420 @@
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <conditionalFormatting sqref="J618:J742 J744 J746 J748 J750 J752 J754 J756 J758 J760:J766 J914:J1037 J1039:J1176 J1181:J1195 J1200:J1204 J1209:J1258 J1262:J1286 J1288:J1380 J1384:J1408 J1410:J1469 J1471:J1557 J1596:J1617 J1754:J1755 J1758:J1785 J1913:J1954 J1957:J1959 J1962 J1964:J1966 J1969:J2006 J2009:J2049 J2052:J2074 J2077:J2080 J2083 J2085:J2087 J2090:J2131 J2327:J65039 O618:O742 O744 O746 O748 O750 O752 O754 O756 O758 O760:O766 O914:O1037 O1039:O1176 O1181:O1195 O1200:O1204 O1209:O1258 O1262:O1286 O1288:O1380 O1384:O1408 O1410:O1469 O1471:O1557 O1596:O1617 O1754:O1755 O1758:O1785 O1913:O1954 O1957:O1959 O1962 O1964:O1966 O1969:O2006 O2009:O2049 O2052:O2074 O2077:O2080 O2083 O2085:O2087 O2090:O2131 O2327:O65039 J9:J11 J23:J601 O9:O601 T11:T601 J18:J21">
-    <cfRule type="cellIs" dxfId="129" priority="238" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="238" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="239" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="239" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="240" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="240" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11 I23:I68 N11:N68 S11:S68 I18:I21">
-    <cfRule type="cellIs" dxfId="126" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="230" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="231" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="232" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="233" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="234" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11 I23:I68 N11:N68 S11:S68 I18:I21">
-    <cfRule type="cellIs" dxfId="121" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="215" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="216" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T618:T742 T744 T746 T748 T750 T752 T754 T756 T758 T760:T766 T914:T1037 T1039:T1176 T1181:T1195 T1200:T1204 T1209:T1258 T1262:T1286 T1288:T1380 T1384:T1408 T1410:T1469 T1471:T1557 T1596:T1617 T1754:T1755 T1758:T1785 T1913:T1954 T1957:T1959 T1962 T1964:T1966 T1969:T2006 T2009:T2049 T2052:T2074 T2077:T2080 T2083 T2085:T2087 T2090:T2131 T2327:T65039 T9:T10">
-    <cfRule type="cellIs" dxfId="119" priority="205" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="205" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="206" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="206" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="207" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="207" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="116" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="163" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="164" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="165" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="166" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="167" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="111" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="161" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="162" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="109" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="153" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="154" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="155" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="156" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="157" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="104" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="151" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="152" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="102" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="143" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="144" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="145" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="146" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="147" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="97" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="141" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="142" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="95" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="123" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="124" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="125" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="126" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="127" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="90" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="121" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="122" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="cellIs" dxfId="88" priority="118" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="118" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="119" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="119" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="120" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="120" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="cellIs" dxfId="85" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="113" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="114" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="115" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="116" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="117" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="cellIs" dxfId="80" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="111" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="112" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="78" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="103" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="104" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="105" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="106" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="107" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="73" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="101" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="102" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="71" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="69" priority="88" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="88" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="89" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="89" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="90" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="90" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="66" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="83" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="84" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="85" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="86" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="87" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="61" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="81" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="82" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="cellIs" dxfId="59" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="78" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="79" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="79" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="80" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="80" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="cellIs" dxfId="56" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="73" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="74" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="75" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="76" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="77" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="51" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="68" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="69" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="70" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="48" priority="62" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="62" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="63" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="63" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="64" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="64" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="45" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="57" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="42" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="54" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="55" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="45" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="46" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="47" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="48" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="49" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="43" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="44" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="35" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="36" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="37" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="39" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="33" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="34" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="cellIs" dxfId="25" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22">
-    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22">
-    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5434,8 +5345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5471,7 +5382,7 @@
         <v>76</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F2" s="40" t="s">
         <v>77</v>
@@ -5504,19 +5415,19 @@
         <v>43753</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -5530,19 +5441,19 @@
         <v>43753</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.2">
@@ -5556,19 +5467,19 @@
         <v>43753</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -5582,22 +5493,22 @@
         <v>43753</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="132" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="108" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>5</v>
       </c>
@@ -5608,19 +5519,19 @@
         <v>43753</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -5634,19 +5545,19 @@
         <v>43753</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.2">
@@ -5660,19 +5571,19 @@
         <v>43753</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.2">
@@ -5686,19 +5597,19 @@
         <v>43753</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.2">
@@ -5712,22 +5623,22 @@
         <v>43753</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="252" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>10</v>
       </c>
@@ -5738,19 +5649,19 @@
         <v>43753</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>167</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>80</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -5830,11 +5741,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5964,20 +5876,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6001,9 +5910,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Template de Casos de Prueba modificado con 1 caso de prueba y 1 error nuevo
</commit_message>
<xml_diff>
--- a/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
+++ b/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Archivos Generales\Facultad\ISW\Repositorio\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\UTN\Ingenieria de Software\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A510E4-87A2-492C-875C-E72D43FAA5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -24,12 +23,12 @@
     <definedName name="Ready_To_Run">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr autoRecover="0"/>
+  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="179">
   <si>
     <t>TC_001</t>
   </si>
@@ -563,36 +562,6 @@
   <si>
     <t>1. El sistema valida si el usuario ingresó o no algo en el campo de "Referencia Opcional".
 2. El sistema valida que el texto ingresado "Edificio con puerta de vidrio ubicado entre un kiosco y una panadería" sea un texto alfanumérico, o solo texto válido, y lo es.</t>
-  </si>
-  <si>
-    <t>1. El usuario ingresa el nombre de calle "598".
-2. El usuario no selecciona valor para el campo "Ciudad" del menú desplegable de Ciudad.
-3. El usuario no selecciona valor para el campo "Provincia" del menú desplegable de Provincia.
-4. El usuario ingresa el valor "aaa" para el campo "ZIP".
-5. El usuario selecciona la opción "Determinar fecha y hora de recepción".
-6. El usuario ingresa la fecha "15/09/2019" como fecha de recepción.
-7. El usuario ingresa la hora "25:00" como hora de recepción.
-8. El usuario selecciona la forma de pago "Tarjeta VISA".
-9. El usuario ingresa el número de tarjeta "0000 1111 2222 3333".
-10. El usuario ingresa nombre y apellido "156".
-11. El usuario ingresa fecha de vencimiento de la tarjeta "04/17".
-12. El usuario ingresa el CVC "0". 
-13. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
-    <t>1. El sistema valida que el nombre de calle "598" sea solo texto, y que sea un nombre válido, y no lo es.
-2. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de Ciudad, que la opción " " sea inválida, y no es así.
-3. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de Pronvincia, que la opción " " sea inválida, y no es así.
-4. El sistema valida que el valor de código postal ingresado "aaa" sea numérico, válido, y no lo es.
-5. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
-6. El sistema valida que la fecha ingresada por el usuario "15/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y es así.
-7. El sistema valida que la hora ingresada por el usuario "22:00" sea una hora con formato válido, mayor a la hora actual, y es así.
-8. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
-9. El sistema valida que el número de tarjeta ingresado por el usuario "0000 1111 2222 3333" sea un número de tarjeta inválido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
-10. El sistema valida que el nombre y apellido "156" sea texto válido, y no lo es.
-11. El sistema valida que la fecha de vencimiento "04/17" sea válida, y no lo es.
-10. El sistema valida que el código CVC "0" ingresado sea inválido, y no lo es.
-13. El sistema muestra el mensaje "Datos erróneos".</t>
   </si>
   <si>
     <t>1. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
@@ -624,11 +593,89 @@
 13. Ingresar un código CVC inválido (por ejemplo, '0').
 14. Seleccionar la opción "Aceptar".</t>
   </si>
+  <si>
+    <t>Grupo 5</t>
+  </si>
+  <si>
+    <t>Realizacion del pedido con fecha programada y en efectivo</t>
+  </si>
+  <si>
+    <t>User Story de Realizar Pedido a Comercio Adherido (Grupo 6)</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el nombre de calle "598" sea solo texto, y que sea un nombre válido, y no lo es.
+2. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de Ciudad, que la opción " " sea inválida, y no es así.
+3. El sistema valida que el usuario haya seleccionado una opción del menú desplegable de Pronvincia, que la opción " " sea inválida, y no es así.
+4. El sistema valida que el valor de código postal ingresado "aaa" sea numérico, válido, y no lo es.
+5. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
+6. El sistema valida que la fecha ingresada por el usuario "15/09/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y no es así.
+7. El sistema valida que la hora ingresada por el usuario "22:00" sea una hora con formato válido, mayor a la hora actual, y es así.
+8. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+9. El sistema valida que el número de tarjeta ingresado por el usuario "0000 1111 2222 3333" sea un número de tarjeta inválido, con la longitud de 16 caracteres y que corresponda a una tarjeta VISA válida, y no corresponde.
+10. El sistema valida que el nombre y apellido "156" sea texto válido, y no lo es.
+11. El sistema valida que la fecha de vencimiento "04/17" sea válida, y no lo es.
+10. El sistema valida que el código CVC "0" ingresado sea inválido, y no lo es.
+13. El sistema muestra el mensaje "Datos erróneos".</t>
+  </si>
+  <si>
+    <t>El usuario debe haber elegido algun producto del comercio adherido y agregado al carrito y agrega una direccion, provincia, ciudad y codigo postal valida</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresa el nombre de calle "598".
+2. El usuario no selecciona valor para el campo "Ciudad" del menú desplegable de Ciudad.
+3. El usuario no selecciona valor para el campo "Provincia" del menú desplegable de Provincia.
+4. El usuario ingresa el valor "aaa" para el campo "ZIP".
+5. El usuario selecciona la opción "Determinar fecha y hora de recepción".
+6. El usuario ingresa la fecha "15/09/2019" como fecha de recepción.
+7. El usuario ingresa la hora "22:00" como hora de recepción.
+8. El usuario selecciona la forma de pago "Tarjeta VISA".
+9. El usuario ingresa el número de tarjeta "0000 1111 2222 3333".
+10. El usuario ingresa nombre y apellido "156".
+11. El usuario ingresa fecha de vencimiento de la tarjeta "04/17".
+12. El usuario ingresa el CVC "0". 
+13. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>El sistema no notifica si hay datos faltantes o si el pedido se registró con éxito por lo cual deja con incertidumbre al usuario acerca del estado del mismo.</t>
+  </si>
+  <si>
+    <t>2019-20-15</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>El sistema no aparenta validar los campos "Fecha deseada", ni "Hora Deseada", ni "Monto de Pago", tampoco si valida el formato correcto de "Fecha Deseada" y "Hora Desada" y tambien si es un numero negativo el "Monto de Pago". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona la opción "Determinar fecha y hora de recepción".
+2. El usuario ingresa la fecha "10/14/2019" como fecha de recepción.
+3. El usuario ingresa la hora "35:20" como hora de recepción.
+4. El usuario selecciona la opcion de forma de pago "Efectivo".
+5. El usuario ingresa el monto de pago de "-300".
+6. El usuario selecciona la opcion "Aceptar"</t>
+  </si>
+  <si>
+    <t>1. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
+2. El sistema valida que la fecha ingresada por el usuario "10/14/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y no es así.
+3. El sistema valida que la hora ingresada por el usuario "35:20" sea una hora con formato válido, mayor a la hora actual, y no es así.
+4. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
+5. El sistema valida que el monto ingresado "-300"  sea mayor o igual al monto del pedio o si es un numero negativo, y no es asi.
+6. El sistema muestra mensaje de "Datos Erroneos"</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Determinar fecha y hora de recepción".
+2. Ingresar una fecha de recepcion con formato "MM/DD/AAA"  y que sea menor a la actual.
+3. Ingresar la hora de recepcion con formato "MM:HH".
+4. Seleccionar la opcion de forma de pago "Efectivo".
+5. Ingresar un numero negativo para el monto de pago.
+6. Seleccionar la opcion "Aceptar".</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -742,7 +789,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,6 +847,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,7 +1067,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1123,6 +1176,9 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1135,7 +1191,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1146,15 +1202,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="DataPilot Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="DataPilot Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="DataPilot Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="DataPilot Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="DataPilot Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="DataPilot Category" xfId="1"/>
+    <cellStyle name="DataPilot Corner" xfId="2"/>
+    <cellStyle name="DataPilot Field" xfId="3"/>
+    <cellStyle name="DataPilot Result" xfId="4"/>
+    <cellStyle name="DataPilot Title" xfId="5"/>
+    <cellStyle name="DataPilot Value" xfId="6"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 2" xfId="8"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="116">
@@ -2441,15 +2497,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2512,14 +2568,14 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
       <c r="I2" s="32"/>
@@ -2547,12 +2603,12 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -2580,12 +2636,12 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -2613,14 +2669,18 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -2674,34 +2734,34 @@
     </row>
     <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="47" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47" t="s">
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47" t="s">
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -3356,10 +3416,10 @@
         <v>153</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>116</v>
@@ -3393,20 +3453,43 @@
       <c r="AR21" s="7"/>
       <c r="AS21" s="7"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" ht="168" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="37"/>
+      <c r="B22" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="K22" s="29">
+        <v>11</v>
+      </c>
+      <c r="L22" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="M22" s="39"/>
       <c r="N22" s="15"/>
       <c r="O22" s="28"/>
@@ -4897,7 +4980,7 @@
       <c r="AS68" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:AS2326" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A9:AS2326"/>
   <mergeCells count="7">
     <mergeCell ref="A2:F4"/>
     <mergeCell ref="H8:L8"/>
@@ -5327,11 +5410,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P62:P63 K62:K63 U62:U63" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I23:I68 S11:S68 N11:N68 I11:I21" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P62:P63 K62:K63 U62:U63"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I23:I68 S11:S68 N11:N68 I11:I21">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B23:B68 B15:B21" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B23:B68 B15:B21">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5342,11 +5425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5482,7 +5565,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>4</v>
       </c>
@@ -5519,10 +5602,10 @@
         <v>43753</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>118</v>
@@ -5649,10 +5732,10 @@
         <v>43753</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>118</v>
@@ -5664,17 +5747,31 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>11</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="B14" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="44">
+        <v>43753</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
@@ -5726,13 +5823,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5741,6 +5838,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5749,7 +5854,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5875,15 +5980,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5891,7 +5998,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5907,14 +6014,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>